<commit_message>
Add date of birth column to Delius test fixture
The sample Delius extract (XLSX) file was missing the 'Date of Birth'
column, so I've added it. This makes it more representative of a
real-world Delius extract file that we'd process in production.
</commit_message>
<xml_diff>
--- a/spec/fixtures/delius/delius_sample.xlsx
+++ b/spec/fixtures/delius/delius_sample.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ollie/moj/offender-management-allocation-manager/spec/fixtures/delius/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E36BB03-F349-E246-A269-03974388E69C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="840" yWindow="460" windowWidth="50360" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="export_test" sheetId="1" r:id="rId3"/>
+    <sheet name="export_test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="145">
   <si>
     <t>CRN</t>
   </si>
@@ -440,64 +449,382 @@
   </si>
   <si>
     <t>G3356GT</t>
+  </si>
+  <si>
+    <t>Birth Dt (O)</t>
+  </si>
+  <si>
+    <t>19/03/1985</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,8 +876,11 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="R1" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -600,10 +930,13 @@
         <v>32</v>
       </c>
       <c r="Q2" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -653,10 +986,13 @@
         <v>24</v>
       </c>
       <c r="Q3" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -706,10 +1042,13 @@
         <v>32</v>
       </c>
       <c r="Q4" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>1</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -759,10 +1098,13 @@
         <v>24</v>
       </c>
       <c r="Q5" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>1</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -812,10 +1154,13 @@
         <v>24</v>
       </c>
       <c r="Q6" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>1</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -865,10 +1210,13 @@
         <v>24</v>
       </c>
       <c r="Q7" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>1</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -918,10 +1266,13 @@
         <v>24</v>
       </c>
       <c r="Q8" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>1</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -971,10 +1322,13 @@
         <v>24</v>
       </c>
       <c r="Q9" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>1</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1024,10 +1378,13 @@
         <v>32</v>
       </c>
       <c r="Q10" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>1</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1074,10 +1431,13 @@
         <v>32</v>
       </c>
       <c r="Q11" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>1</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1127,10 +1487,13 @@
         <v>24</v>
       </c>
       <c r="Q12" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>1</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1180,10 +1543,13 @@
         <v>24</v>
       </c>
       <c r="Q13" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>1</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -1233,10 +1599,13 @@
         <v>24</v>
       </c>
       <c r="Q14" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>1</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1286,10 +1655,13 @@
         <v>32</v>
       </c>
       <c r="Q15" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>1</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1339,10 +1711,13 @@
         <v>24</v>
       </c>
       <c r="Q16" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>1</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1392,10 +1767,13 @@
         <v>32</v>
       </c>
       <c r="Q17" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>1</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1442,10 +1820,13 @@
         <v>32</v>
       </c>
       <c r="Q18" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>1</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1495,10 +1876,13 @@
         <v>32</v>
       </c>
       <c r="Q19" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>1</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1548,10 +1932,13 @@
         <v>24</v>
       </c>
       <c r="Q20" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>1</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -1601,10 +1988,13 @@
         <v>32</v>
       </c>
       <c r="Q21" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>1</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -1654,10 +2044,13 @@
         <v>24</v>
       </c>
       <c r="Q22" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>1</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1707,10 +2100,13 @@
         <v>32</v>
       </c>
       <c r="Q23" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>1</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -1760,10 +2156,13 @@
         <v>32</v>
       </c>
       <c r="Q24" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>1</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -1813,10 +2212,13 @@
         <v>32</v>
       </c>
       <c r="Q25" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>1</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
@@ -1866,10 +2268,13 @@
         <v>32</v>
       </c>
       <c r="Q26" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>1</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
@@ -1919,10 +2324,13 @@
         <v>24</v>
       </c>
       <c r="Q27" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>1</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
@@ -1972,10 +2380,13 @@
         <v>24</v>
       </c>
       <c r="Q28" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>1</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
@@ -2025,10 +2436,13 @@
         <v>32</v>
       </c>
       <c r="Q29" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>1</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
@@ -2078,10 +2492,13 @@
         <v>32</v>
       </c>
       <c r="Q30" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>1</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
@@ -2131,10 +2548,13 @@
         <v>24</v>
       </c>
       <c r="Q31" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>1</v>
+      </c>
+      <c r="R31" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
@@ -2184,10 +2604,13 @@
         <v>32</v>
       </c>
       <c r="Q32" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>1</v>
+      </c>
+      <c r="R32" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
@@ -2237,10 +2660,13 @@
         <v>24</v>
       </c>
       <c r="Q33" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>1</v>
+      </c>
+      <c r="R33" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -2290,10 +2716,13 @@
         <v>24</v>
       </c>
       <c r="Q34" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>1</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
@@ -2343,10 +2772,13 @@
         <v>24</v>
       </c>
       <c r="Q35" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>1</v>
+      </c>
+      <c r="R35" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>17</v>
       </c>
@@ -2396,10 +2828,13 @@
         <v>24</v>
       </c>
       <c r="Q36" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>1</v>
+      </c>
+      <c r="R36" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
@@ -2449,10 +2884,13 @@
         <v>32</v>
       </c>
       <c r="Q37" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>1</v>
+      </c>
+      <c r="R37" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>17</v>
       </c>
@@ -2502,10 +2940,13 @@
         <v>24</v>
       </c>
       <c r="Q38" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>1</v>
+      </c>
+      <c r="R38" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>17</v>
       </c>
@@ -2555,10 +2996,13 @@
         <v>32</v>
       </c>
       <c r="Q39" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>1</v>
+      </c>
+      <c r="R39" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -2608,10 +3052,13 @@
         <v>24</v>
       </c>
       <c r="Q40" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>1</v>
+      </c>
+      <c r="R40" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -2661,10 +3108,13 @@
         <v>32</v>
       </c>
       <c r="Q41" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>1</v>
+      </c>
+      <c r="R41" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
@@ -2714,10 +3164,13 @@
         <v>32</v>
       </c>
       <c r="Q42" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>1</v>
+      </c>
+      <c r="R42" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
@@ -2767,10 +3220,13 @@
         <v>24</v>
       </c>
       <c r="Q43" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>1</v>
+      </c>
+      <c r="R43" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>17</v>
       </c>
@@ -2820,10 +3276,13 @@
         <v>32</v>
       </c>
       <c r="Q44" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>1</v>
+      </c>
+      <c r="R44" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>17</v>
       </c>
@@ -2873,10 +3332,13 @@
         <v>32</v>
       </c>
       <c r="Q45" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>1</v>
+      </c>
+      <c r="R45" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
@@ -2926,10 +3388,13 @@
         <v>32</v>
       </c>
       <c r="Q46" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>1</v>
+      </c>
+      <c r="R46" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>17</v>
       </c>
@@ -2979,10 +3444,13 @@
         <v>32</v>
       </c>
       <c r="Q47" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>1</v>
+      </c>
+      <c r="R47" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>17</v>
       </c>
@@ -3032,10 +3500,13 @@
         <v>24</v>
       </c>
       <c r="Q48" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>1</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>17</v>
       </c>
@@ -3085,10 +3556,13 @@
         <v>24</v>
       </c>
       <c r="Q49" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>1</v>
+      </c>
+      <c r="R49" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>17</v>
       </c>
@@ -3138,10 +3612,13 @@
         <v>24</v>
       </c>
       <c r="Q50" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>1</v>
+      </c>
+      <c r="R50" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>17</v>
       </c>
@@ -3191,10 +3668,13 @@
         <v>24</v>
       </c>
       <c r="Q51" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>1</v>
+      </c>
+      <c r="R51" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>17</v>
       </c>
@@ -3244,10 +3724,13 @@
         <v>32</v>
       </c>
       <c r="Q52" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>1</v>
+      </c>
+      <c r="R52" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>17</v>
       </c>
@@ -3297,10 +3780,13 @@
         <v>32</v>
       </c>
       <c r="Q53" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>1</v>
+      </c>
+      <c r="R53" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>17</v>
       </c>
@@ -3350,10 +3836,13 @@
         <v>24</v>
       </c>
       <c r="Q54" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="55">
+        <v>1</v>
+      </c>
+      <c r="R54" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>17</v>
       </c>
@@ -3403,10 +3892,13 @@
         <v>24</v>
       </c>
       <c r="Q55" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="56">
+        <v>1</v>
+      </c>
+      <c r="R55" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>17</v>
       </c>
@@ -3456,10 +3948,13 @@
         <v>32</v>
       </c>
       <c r="Q56" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="57">
+        <v>1</v>
+      </c>
+      <c r="R56" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>17</v>
       </c>
@@ -3506,10 +4001,13 @@
         <v>24</v>
       </c>
       <c r="Q57" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="58">
+        <v>1</v>
+      </c>
+      <c r="R57" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>17</v>
       </c>
@@ -3559,10 +4057,13 @@
         <v>32</v>
       </c>
       <c r="Q58" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>1</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>17</v>
       </c>
@@ -3612,10 +4113,13 @@
         <v>32</v>
       </c>
       <c r="Q59" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>1</v>
+      </c>
+      <c r="R59" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>17</v>
       </c>
@@ -3665,10 +4169,13 @@
         <v>32</v>
       </c>
       <c r="Q60" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>1</v>
+      </c>
+      <c r="R60" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>17</v>
       </c>
@@ -3718,10 +4225,13 @@
         <v>32</v>
       </c>
       <c r="Q61" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="62">
+        <v>1</v>
+      </c>
+      <c r="R61" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>17</v>
       </c>
@@ -3771,10 +4281,13 @@
         <v>32</v>
       </c>
       <c r="Q62" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="63">
+        <v>1</v>
+      </c>
+      <c r="R62" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>17</v>
       </c>
@@ -3824,10 +4337,13 @@
         <v>24</v>
       </c>
       <c r="Q63" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="64">
+        <v>1</v>
+      </c>
+      <c r="R63" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>17</v>
       </c>
@@ -3877,10 +4393,13 @@
         <v>32</v>
       </c>
       <c r="Q64" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="65">
+        <v>1</v>
+      </c>
+      <c r="R64" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>17</v>
       </c>
@@ -3930,10 +4449,13 @@
         <v>24</v>
       </c>
       <c r="Q65" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="66">
+        <v>1</v>
+      </c>
+      <c r="R65" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
         <v>17</v>
       </c>
@@ -3980,10 +4502,13 @@
         <v>24</v>
       </c>
       <c r="Q66" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="67">
+        <v>1</v>
+      </c>
+      <c r="R66" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>17</v>
       </c>
@@ -4033,10 +4558,13 @@
         <v>32</v>
       </c>
       <c r="Q67" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="68">
+        <v>1</v>
+      </c>
+      <c r="R67" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>17</v>
       </c>
@@ -4086,10 +4614,13 @@
         <v>24</v>
       </c>
       <c r="Q68" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="69">
+        <v>1</v>
+      </c>
+      <c r="R68" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>17</v>
       </c>
@@ -4139,10 +4670,13 @@
         <v>24</v>
       </c>
       <c r="Q69" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>1</v>
+      </c>
+      <c r="R69" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>17</v>
       </c>
@@ -4192,10 +4726,13 @@
         <v>32</v>
       </c>
       <c r="Q70" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="71">
+        <v>1</v>
+      </c>
+      <c r="R70" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>17</v>
       </c>
@@ -4245,10 +4782,13 @@
         <v>24</v>
       </c>
       <c r="Q71" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="72">
+        <v>1</v>
+      </c>
+      <c r="R71" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>17</v>
       </c>
@@ -4295,10 +4835,13 @@
         <v>32</v>
       </c>
       <c r="Q72" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="73">
+        <v>1</v>
+      </c>
+      <c r="R72" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>17</v>
       </c>
@@ -4348,10 +4891,13 @@
         <v>24</v>
       </c>
       <c r="Q73" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="74">
+        <v>1</v>
+      </c>
+      <c r="R73" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
         <v>17</v>
       </c>
@@ -4398,10 +4944,13 @@
         <v>24</v>
       </c>
       <c r="Q74" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="75">
+        <v>1</v>
+      </c>
+      <c r="R74" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
         <v>17</v>
       </c>
@@ -4451,10 +5000,13 @@
         <v>24</v>
       </c>
       <c r="Q75" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="76">
+        <v>1</v>
+      </c>
+      <c r="R75" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>17</v>
       </c>
@@ -4504,10 +5056,13 @@
         <v>32</v>
       </c>
       <c r="Q76" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="77">
+        <v>1</v>
+      </c>
+      <c r="R76" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
         <v>17</v>
       </c>
@@ -4557,10 +5112,13 @@
         <v>24</v>
       </c>
       <c r="Q77" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="78">
+        <v>1</v>
+      </c>
+      <c r="R77" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
         <v>17</v>
       </c>
@@ -4610,10 +5168,13 @@
         <v>24</v>
       </c>
       <c r="Q78" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="79">
+        <v>1</v>
+      </c>
+      <c r="R78" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
         <v>17</v>
       </c>
@@ -4663,10 +5224,13 @@
         <v>24</v>
       </c>
       <c r="Q79" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="80">
+        <v>1</v>
+      </c>
+      <c r="R79" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
         <v>17</v>
       </c>
@@ -4716,10 +5280,13 @@
         <v>32</v>
       </c>
       <c r="Q80" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="81">
+        <v>1</v>
+      </c>
+      <c r="R80" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
         <v>17</v>
       </c>
@@ -4769,10 +5336,13 @@
         <v>32</v>
       </c>
       <c r="Q81" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="82">
+        <v>1</v>
+      </c>
+      <c r="R81" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
         <v>17</v>
       </c>
@@ -4822,10 +5392,13 @@
         <v>24</v>
       </c>
       <c r="Q82" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="83">
+        <v>1</v>
+      </c>
+      <c r="R82" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
         <v>17</v>
       </c>
@@ -4875,10 +5448,13 @@
         <v>24</v>
       </c>
       <c r="Q83" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="84">
+        <v>1</v>
+      </c>
+      <c r="R83" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
         <v>17</v>
       </c>
@@ -4928,10 +5504,13 @@
         <v>32</v>
       </c>
       <c r="Q84" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="85">
+        <v>1</v>
+      </c>
+      <c r="R84" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
         <v>17</v>
       </c>
@@ -4981,10 +5560,13 @@
         <v>32</v>
       </c>
       <c r="Q85" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="86">
+        <v>1</v>
+      </c>
+      <c r="R85" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
         <v>17</v>
       </c>
@@ -5034,10 +5616,13 @@
         <v>32</v>
       </c>
       <c r="Q86" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="87">
+        <v>1</v>
+      </c>
+      <c r="R86" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
         <v>17</v>
       </c>
@@ -5087,10 +5672,13 @@
         <v>32</v>
       </c>
       <c r="Q87" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="88">
+        <v>1</v>
+      </c>
+      <c r="R87" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
         <v>17</v>
       </c>
@@ -5140,10 +5728,13 @@
         <v>24</v>
       </c>
       <c r="Q88" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="89">
+        <v>1</v>
+      </c>
+      <c r="R88" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
         <v>17</v>
       </c>
@@ -5193,10 +5784,13 @@
         <v>32</v>
       </c>
       <c r="Q89" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="90">
+        <v>1</v>
+      </c>
+      <c r="R89" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
         <v>17</v>
       </c>
@@ -5246,10 +5840,13 @@
         <v>24</v>
       </c>
       <c r="Q90" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="91">
+        <v>1</v>
+      </c>
+      <c r="R90" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
         <v>17</v>
       </c>
@@ -5299,10 +5896,13 @@
         <v>32</v>
       </c>
       <c r="Q91" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="92">
+        <v>1</v>
+      </c>
+      <c r="R91" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
         <v>17</v>
       </c>
@@ -5352,10 +5952,13 @@
         <v>24</v>
       </c>
       <c r="Q92" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="93">
+        <v>1</v>
+      </c>
+      <c r="R92" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
         <v>17</v>
       </c>
@@ -5405,10 +6008,13 @@
         <v>24</v>
       </c>
       <c r="Q93" s="1">
-        <v>1.0</v>
+        <v>1</v>
+      </c>
+      <c r="R93" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implement new Delius extract file reader
This commit implements a new Delius extract file reader
`Delius::ExtractFileReader` which is intended to replace
`Delius::Processor`.

`Delius::ExtractFileReader` reads the Delius XLSX file using `roo` gem,
whereas `Delius::Processor` implemented a custom XLSX reader. This
sidesteps a bug which existed in the custom XLSX reader implementation
where cells containing ampersands were read incorrectly.

`Delius::ExtractFileReader` also returns Delius records as Hash objects,
where the cell values have been mapped to field names. This will allow
us to DRY-up our codebase – this key => value mapping is currently
being performed is 3 separate parts of our codebase, and this will
remove the need for those.
</commit_message>
<xml_diff>
--- a/spec/fixtures/delius/delius_sample.xlsx
+++ b/spec/fixtures/delius/delius_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ollie/moj/offender-management-allocation-manager/spec/fixtures/delius/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E36BB03-F349-E246-A269-03974388E69C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A2E10E-4B8D-0E42-81E2-A2BD4565DD9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="460" windowWidth="50360" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="149">
   <si>
     <t>CRN</t>
   </si>
@@ -455,6 +455,18 @@
   </si>
   <si>
     <t>19/03/1985</t>
+  </si>
+  <si>
+    <t>Norfolk &amp; Suffolk LDU</t>
+  </si>
+  <si>
+    <t>LDNNCAI</t>
+  </si>
+  <si>
+    <t>N&amp;S-Bury St Edmunds</t>
+  </si>
+  <si>
+    <t>N06208</t>
   </si>
 </sst>
 </file>
@@ -819,7 +831,7 @@
   <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1027,16 +1039,16 @@
         <v>34</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>37</v>
+        <v>145</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>31</v>
+        <v>148</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>32</v>
@@ -6016,5 +6028,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>